<commit_message>
add new and modified files
</commit_message>
<xml_diff>
--- a/Airbnb_Earnings_Expenses_Oaklands.xlsx
+++ b/Airbnb_Earnings_Expenses_Oaklands.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glads\Downloads\OAKLANDS-GUESTS-GOOLESHEETS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478DA7F3-06AE-4104-BE40-C59779A70060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -77,13 +83,25 @@
   </si>
   <si>
     <t>January</t>
+  </si>
+  <si>
+    <t>Rai Davis</t>
+  </si>
+  <si>
+    <t>Townhouse</t>
+  </si>
+  <si>
+    <t>Rai Davis pdf</t>
+  </si>
+  <si>
+    <t>July</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,24 +153,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -190,7 +218,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -224,6 +252,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -258,9 +287,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -433,14 +463,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -504,7 +547,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -534,6 +577,35 @@
       </c>
       <c r="J3" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>45854</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45842</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45846</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5">
+        <v>318.48</v>
+      </c>
+      <c r="H5">
+        <v>275.99</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>